<commit_message>
changed composition 26th january
</commit_message>
<xml_diff>
--- a/src/AlgoComposition.xlsx
+++ b/src/AlgoComposition.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2020old" sheetId="1" state="visible" r:id="rId3"/>
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'2015'!$A$1:$E$37</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'2020'!$A$1:$E$36</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'2020'!$A$1:$E$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="86">
   <si>
     <t xml:space="preserve">Symbol</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t xml:space="preserve">Micron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robinhood Markets Inc</t>
   </si>
   <si>
     <t xml:space="preserve">COST</t>
@@ -381,7 +387,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -389,17 +395,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -408,19 +414,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,11 +434,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,12 +446,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Pivot Table Field" xfId="20"/>
+    <cellStyle name="Pivot Table Category" xfId="20"/>
     <cellStyle name="Pivot Table Corner" xfId="21"/>
-    <cellStyle name="Pivot Table Value" xfId="22"/>
-    <cellStyle name="Pivot Table Category" xfId="23"/>
+    <cellStyle name="Pivot Table Field" xfId="22"/>
+    <cellStyle name="Pivot Table Result" xfId="23"/>
     <cellStyle name="Pivot Table Title" xfId="24"/>
-    <cellStyle name="Pivot Table Result" xfId="25"/>
+    <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -585,7 +587,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C2:C8 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -755,7 +757,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -921,15 +923,15 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="C2:C8 C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,7 +965,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -981,7 +983,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -999,7 +1001,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1017,7 +1019,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1035,7 +1037,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1053,16 +1055,16 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>45993</v>
+        <v>46048</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>55146</v>
@@ -1071,49 +1073,49 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>22</v>
+      <c r="E8" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>45903</v>
+        <v>45993</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>45992</v>
+        <v>46047</v>
       </c>
       <c r="D9" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>27</v>
+      <c r="E9" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>45931</v>
+        <v>45903</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>45964</v>
+        <v>45992</v>
       </c>
       <c r="D10" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>19</v>
+      <c r="E10" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>45931</v>
@@ -1125,8 +1127,8 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>29</v>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,25 +1136,25 @@
         <v>30</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>45778</v>
+        <v>45931</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>45930</v>
+        <v>45964</v>
       </c>
       <c r="D12" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>30</v>
+      <c r="E12" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>45839</v>
+        <v>45778</v>
       </c>
       <c r="C13" s="5" t="n">
         <v>45930</v>
@@ -1161,7 +1163,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1179,7 +1181,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1197,7 +1199,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1206,22 +1208,22 @@
         <v>37</v>
       </c>
       <c r="B16" s="5" t="n">
-        <v>45870</v>
+        <v>45839</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>45902</v>
+        <v>45930</v>
       </c>
       <c r="D16" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>37</v>
+      <c r="E16" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>45870</v>
@@ -1233,7 +1235,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1242,25 +1244,25 @@
         <v>40</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>45692</v>
+        <v>45870</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>45869</v>
+        <v>45902</v>
       </c>
       <c r="D18" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>45653</v>
+        <v>45692</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>45869</v>
@@ -1269,34 +1271,34 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>6</v>
+      <c r="E19" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B20" s="5" t="n">
-        <v>45748</v>
+        <v>45653</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>45838</v>
+        <v>45869</v>
       </c>
       <c r="D20" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>42</v>
+      <c r="E20" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>45778</v>
+        <v>45748</v>
       </c>
       <c r="C21" s="5" t="n">
         <v>45838</v>
@@ -1305,7 +1307,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1314,7 +1316,7 @@
         <v>45</v>
       </c>
       <c r="B22" s="5" t="n">
-        <v>45811</v>
+        <v>45778</v>
       </c>
       <c r="C22" s="5" t="n">
         <v>45838</v>
@@ -1323,7 +1325,7 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1332,43 +1334,43 @@
         <v>47</v>
       </c>
       <c r="B23" s="5" t="n">
-        <v>45778</v>
+        <v>45811</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>45810</v>
+        <v>45838</v>
       </c>
       <c r="D23" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>47</v>
+      <c r="E23" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B24" s="5" t="n">
-        <v>45748</v>
+        <v>45778</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>45777</v>
+        <v>45810</v>
       </c>
       <c r="D24" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>14</v>
+      <c r="E24" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B25" s="5" t="n">
-        <v>45692</v>
+        <v>45748</v>
       </c>
       <c r="C25" s="5" t="n">
         <v>45777</v>
@@ -1377,8 +1379,8 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>49</v>
+      <c r="E25" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,7 +1388,7 @@
         <v>50</v>
       </c>
       <c r="B26" s="5" t="n">
-        <v>45748</v>
+        <v>45692</v>
       </c>
       <c r="C26" s="5" t="n">
         <v>45777</v>
@@ -1395,31 +1397,31 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5" t="n">
-        <v>45653</v>
+        <v>45748</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>45747</v>
+        <v>45777</v>
       </c>
       <c r="D27" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>24</v>
+      <c r="E27" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>45653</v>
@@ -1431,16 +1433,16 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>53</v>
+      <c r="E28" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="n">
-        <v>45660</v>
+        <v>45653</v>
       </c>
       <c r="C29" s="5" t="n">
         <v>45747</v>
@@ -1449,13 +1451,13 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>32</v>
+      <c r="E29" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>45660</v>
@@ -1467,31 +1469,31 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>36</v>
+      <c r="E30" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>45660</v>
       </c>
       <c r="C31" s="5" t="n">
-        <v>45691</v>
+        <v>45747</v>
       </c>
       <c r="D31" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>55</v>
+      <c r="E31" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>45660</v>
@@ -1503,31 +1505,31 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>10</v>
+      <c r="E32" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B33" s="5" t="n">
-        <v>45653</v>
+        <v>45660</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>45659</v>
+        <v>45691</v>
       </c>
       <c r="D33" s="6" t="n">
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>18</v>
+      <c r="E33" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B34" s="5" t="n">
         <v>45653</v>
@@ -1539,13 +1541,13 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>16</v>
+      <c r="E34" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>45653</v>
@@ -1557,13 +1559,13 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>19</v>
+      <c r="E35" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>45653</v>
@@ -1575,13 +1577,27 @@
         <f aca="false">1/7</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>57</v>
+      <c r="E36" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>45653</v>
+      </c>
+      <c r="C37" s="5" t="n">
+        <v>45659</v>
+      </c>
+      <c r="D37" s="6" t="n">
+        <f aca="false">1/7</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
@@ -1660,7 +1676,7 @@
       <c r="B56" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E36"/>
+  <autoFilter ref="A1:E37"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1679,16 +1695,16 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,7 +1720,7 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1719,7 +1735,7 @@
         <v>55146</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E2" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1791,7 +1807,7 @@
         <v>55146</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1809,7 +1825,7 @@
         <v>55146</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E7" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1836,7 +1852,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>45903</v>
@@ -1845,7 +1861,7 @@
         <v>45992</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E9" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1854,7 +1870,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>45903</v>
@@ -1863,7 +1879,7 @@
         <v>45992</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E10" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1872,7 +1888,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>45931</v>
@@ -1881,7 +1897,7 @@
         <v>45964</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E11" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1890,7 +1906,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>45839</v>
@@ -1899,7 +1915,7 @@
         <v>45930</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1908,7 +1924,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>45839</v>
@@ -1917,7 +1933,7 @@
         <v>45930</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E13" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1926,7 +1942,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>45839</v>
@@ -1935,7 +1951,7 @@
         <v>45930</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E14" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1944,7 +1960,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>45839</v>
@@ -1953,7 +1969,7 @@
         <v>45930</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E15" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1962,7 +1978,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>45870</v>
@@ -1971,7 +1987,7 @@
         <v>45902</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E16" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1980,7 +1996,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>45870</v>
@@ -1989,7 +2005,7 @@
         <v>45902</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E17" s="6" t="n">
         <f aca="false">1/7</f>
@@ -1998,7 +2014,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>45748</v>
@@ -2007,7 +2023,7 @@
         <v>45869</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E18" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2025,7 +2041,7 @@
         <v>45869</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E19" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2034,7 +2050,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="n">
         <v>45778</v>
@@ -2043,7 +2059,7 @@
         <v>45838</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E20" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2052,7 +2068,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21" s="5" t="n">
         <v>45778</v>
@@ -2061,7 +2077,7 @@
         <v>45838</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E21" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2070,7 +2086,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B22" s="5" t="n">
         <v>45778</v>
@@ -2079,7 +2095,7 @@
         <v>45838</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E22" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2088,7 +2104,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B23" s="5" t="n">
         <v>45811</v>
@@ -2097,7 +2113,7 @@
         <v>45838</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E23" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2106,7 +2122,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B24" s="5" t="n">
         <v>45748</v>
@@ -2115,7 +2131,7 @@
         <v>45810</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E24" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2124,7 +2140,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B25" s="5" t="n">
         <v>45692</v>
@@ -2133,7 +2149,7 @@
         <v>45777</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E25" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2142,7 +2158,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>45748</v>
@@ -2151,7 +2167,7 @@
         <v>45777</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E26" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2160,7 +2176,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>45748</v>
@@ -2169,7 +2185,7 @@
         <v>45777</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E27" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2187,7 +2203,7 @@
         <v>45747</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E28" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2196,7 +2212,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>45653</v>
@@ -2205,7 +2221,7 @@
         <v>45747</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E29" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2214,7 +2230,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>45660</v>
@@ -2223,7 +2239,7 @@
         <v>45747</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E30" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2232,7 +2248,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>45660</v>
@@ -2241,7 +2257,7 @@
         <v>45747</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E31" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2250,7 +2266,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>45660</v>
@@ -2259,7 +2275,7 @@
         <v>45747</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E32" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2268,7 +2284,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>45660</v>
@@ -2277,7 +2293,7 @@
         <v>45691</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E33" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2304,7 +2320,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>45653</v>
@@ -2313,7 +2329,7 @@
         <v>45659</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E35" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2322,7 +2338,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>45653</v>
@@ -2331,7 +2347,7 @@
         <v>45659</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E36" s="6" t="n">
         <f aca="false">1/7</f>
@@ -2340,7 +2356,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>45653</v>
@@ -2349,7 +2365,7 @@
         <v>45659</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E37" s="6" t="n">
         <f aca="false">1/7</f>

</xml_diff>